<commit_message>
merge google drive infos
</commit_message>
<xml_diff>
--- a/java.xlsx
+++ b/java.xlsx
@@ -11,26 +11,122 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
-  <si>
-    <t>Language</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+  <si>
+    <t>GSON</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>class BagOfPrimitives {
+  private int value1 = 1;
+  private String value2 = "abc";
+  private transient int value3 = 3;
+  BagOfPrimitives() {
+    // no-args constructor
+  }
+}
+// Serialization
+BagOfPrimitives obj = new BagOfPrimitives();
+Gson gson = new Gson();
+String json = gson.toJson(obj);  
+// Deserialization
+BagOfPrimitives obj2 = gson.fromJson(json, BagOfPrimitives.class);
+// ==&gt; obj2 is just like obj</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Desc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anonymous Inner Class</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>read a file</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>How to run a executable jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>build a java project</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>import project to eclipse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>build a web project</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic command</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read JSON from HttpRequest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write JSON to HttpResponse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cope api</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. java -jar *.jar {argus} : 直接針對該JAR調用MAIN
+2. java -classpath *.jar com.*.*.* : 曲折地把該JAR加為CP, 然後用CP概念調用任一包含STATIC方法的類</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">$/etc/init.d/$ sudo ./tomcat6 start
+$/etc/init.d/$ sudo ./tomcat6 stop
+$/etc/init.d/$ sudo ./tomcat6 restart </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">import org.json.simple.JSONArray;
+import org.json.simple.JSONObject;
+import org.json.simple.parser.JSONParser;
+...
+public void doPost(HttpServletRequest request, HttpServletResponse response)
+  throws ServletException, IOException {
+  StringBuffer jb = new StringBuffer();
+  String line = null;
+  try {
+    BufferedReader reader = request.getReader();
+    while ((line = reader.readLine()) != null)
+      jb.append(line);
+  } catch (Exception e) { /*report an error*/ }
+  try {
+    JSONObject jsonObject = JSONObject.fromObject(jb.toString());
+  } catch (ParseException e) {
+    // crash and burn
+    throw new IOException("Error parsing JSON request string");
+  }
+  // Work with the data using methods like...
+  // int someInt = jsonObject.getInt("intParamName");
+  // String someString = jsonObject.getString("stringParamName");
+  // JSONObject nestedObj = jsonObject.getJSONObject("nestedObjName");
+  // JSONArray arr = jsonObject.getJSONArray("arrayParamName");
+  // etc...
+}
+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Code Ref</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>Anonymous Inner Class</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>JButton testButton = new JButton("Test Button");
@@ -39,28 +135,12 @@
         System.out.println("Click Detected by Anon Class");
     }
 });</t>
-  </si>
-  <si>
-    <t>Apache common io</t>
-  </si>
-  <si>
-    <t>read a file</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>import org.apache.commona.io.FileUtils;
 String fileContent=FileUtils.readFileToString(file);</t>
-  </si>
-  <si>
-    <t>java</t>
-  </si>
-  <si>
-    <t>How to run a executable jar</t>
-  </si>
-  <si>
-    <t>Maven</t>
-  </si>
-  <si>
-    <t>build a java project</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>$ mvn archetype:generate 
@@ -68,18 +148,14 @@
         -DartifactId=my-app 
         -DarchetypeArtifactId=maven-archetype-quickstart 
         -DinteractiveMode=false</t>
-  </si>
-  <si>
-    <t>import project to eclipse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>1. Generate necessary config file for eclipse:
 $mvn eclipse:eclipse -Dwtpversion=2.0
 2. Imports it into Eclipse IDE
 File -&gt; Import… -&gt; General -&gt; Existing Projects into workspace</t>
-  </si>
-  <si>
-    <t>build a web project</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>$ mvn archetype:generate 
@@ -87,29 +163,89 @@
         -DartifactId={project-name} 
         -DarchetypeArtifactId=maven-archetype-webapp 
         -DinteractiveMode=false</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache common io</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>java</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maven</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maven</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Tomcat</t>
-  </si>
-  <si>
-    <t>basic command</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$/etc/init.d/$ sudo ./tomcat6 start
-$/etc/init.d/$ sudo ./tomcat6 stop
-$/etc/init.d/$ sudo ./tomcat6 restart </t>
-  </si>
-  <si>
-    <t>1. java -jar *.jar {argus} : 直接針對該JAR調用MAIN
-2. java -classpath *.jar com.*.*.* : 曲折地把該JAR加為CP, 然後用CP概念調用任一包含STATIC方法的類</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>J2EE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>J2EE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSON</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Language</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>maven repo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;dependencies&gt;
+    &lt;!--  Gson: Java to Json conversion --&gt;
+    &lt;dependency&gt;
+      &lt;groupId&gt;com.google.code.gson&lt;/groupId&gt;
+      &lt;artifactId&gt;gson&lt;/artifactId&gt;
+      &lt;version&gt;2.6.2&lt;/version&gt;
+      &lt;scope&gt;compile&lt;/scope&gt;
+    &lt;/dependency&gt;
+&lt;/dependencies&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>response.setContentType("text/x-json;charset=UTF-8");           
+response.setHeader("Cache-Control", "no-cache");
+response.getWriter().write(json.toString());
+OR
+json.write(response.getWriter());
+OR
+response.getWriter().print(jsonObject);
+response.getWriter().flush();</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regex</t>
+  </si>
+  <si>
+    <t>Pattern p= new Pattern("[abc]");
+Matcher m=p.getMatcher("subject");
+Boolean result= m.matches();</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +274,11 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -165,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -177,6 +318,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -480,112 +624,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>